<commit_message>
Develop Conversation bot with Agentic capabilities and integerate it in FASTAPI backend
</commit_message>
<xml_diff>
--- a/tickets.xlsx
+++ b/tickets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,50 +451,30 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>category</t>
+          <t>raw_incident</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sub_category</t>
+          <t>AI_Incident_summary</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>severity</t>
+          <t>assigned_engineer</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>raw_incident</t>
+          <t>status</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>AI_Incident_summary</t>
+          <t>Engineer_Updates</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>assigned_engineer</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>sla_hours</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Engineer_Updates</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>closing_time</t>
         </is>
@@ -503,12 +483,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TCK-C84DA18B</t>
+          <t>TCK-EFABAF75</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-12-29 05:16:37</t>
+          <t>2026-01-02 09:55:45</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -518,39 +498,34 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>INCIDENT</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Incident Title:
+Incident Description:
+Gross sales margin discrepancy in Power BI report SEF_ALL (production). Observed today. Business impact: Director needs accurate sales figures for closing period. Urgent.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Summarized Mail in Description</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Incident Title:
-Issue in PowerBI Report for SEFPRO
-Incident Description:
-Do we have an update on Ticket : INCSD231234. What is the root cause ? May i Know please ?</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>OPEN</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TCK-311CE4EA</t>
+          <t>TCK-677FB46A</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-29 05:29:54</t>
+          <t>2026-01-02 10:13:38</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -560,33 +535,98 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>INCIDENT</t>
+          <t>Incident Title:
+Incident Description:
+Gross sales margin discrepancy in Power BI report SEF_ALL (production). Observed today. Business impact: Director needs accurate sales figures for closing period. Urgent.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>PowerBI Data Issue</t>
+          <t>Summarized Mail in Description</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Incident Title:
-Issue in PowerBI Report for SEFPRO
-Incident Description:
-Hello Team, I recently noticed an issue where the aggregated 'gross sales by business' in the SEFPRO consolidated Sales Report, is not behaving properly. I can see that the sales for December is increased by 3x. Could you check on this please ?.</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TCK-48A837EA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-01-02 10:13:41</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Incident Title:
+Incident Description:
+Gross sales margin discrepancy in Power BI report SEF_ALL (production). Observed today. Business impact: Director needs accurate sales figures for closing period. Urgent.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Summarized Mail in Description</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>OPEN</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TCK-2F7D24EA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-01-02 10:41:42</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Incident Title:
+Incident Description:
+Incident: Gross sales margin discrepancy in Consolidated Sales Report. System: Azure Synapse. Environment: Production. Noticed this morning. Business impact: None reported. Urgency: Director needs figures for closing period. Request immediate investigation.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Summarized Mail in Description</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>